<commit_message>
fix: formato de df
</commit_message>
<xml_diff>
--- a/data/DataPaper.xlsx
+++ b/data/DataPaper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e64e3084cf54c9d/Documentos/Semestre 6/Contingencias/Proyecto/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B8DC6B5-3383-4515-BA24-2F3A5FA7F2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{6B8DC6B5-3383-4515-BA24-2F3A5FA7F2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E2F6ED-E919-4E0D-8115-AAD735431E3D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B7CE637-673D-40E1-A494-162841D624D0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{3B7CE637-673D-40E1-A494-162841D624D0}"/>
   </bookViews>
   <sheets>
     <sheet name="MaleProb" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="513">
   <si>
     <t>20</t>
   </si>
@@ -431,9 +431,6 @@
   </si>
   <si>
     <t>0.105596</t>
-  </si>
-  <si>
-    <t>Profound</t>
   </si>
   <si>
     <t>0.05</t>
@@ -1977,15 +1974,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B846661C-FC50-46FE-8157-942ED579E486}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:G2"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
@@ -1997,15 +1994,15 @@
         <v>102</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>143</v>
+      <c r="A2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2170,8 +2167,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>49</v>
+      <c r="A10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2336,8 +2333,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>79</v>
+      <c r="A18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -2502,8 +2499,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>102</v>
+      <c r="A26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2668,8 +2665,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>125</v>
+      <c r="A34">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2686,13 +2683,13 @@
         <v>80</v>
       </c>
       <c r="E35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" t="s">
         <v>126</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>127</v>
-      </c>
-      <c r="G35" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2709,13 +2706,13 @@
         <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F36" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" t="s">
         <v>129</v>
-      </c>
-      <c r="G36" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2732,13 +2729,13 @@
         <v>80</v>
       </c>
       <c r="E37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" t="s">
         <v>131</v>
-      </c>
-      <c r="G37" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2755,13 +2752,13 @@
         <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F38" t="s">
+        <v>132</v>
+      </c>
+      <c r="G38" t="s">
         <v>133</v>
-      </c>
-      <c r="G38" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2778,13 +2775,13 @@
         <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" t="s">
         <v>135</v>
-      </c>
-      <c r="G39" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2801,13 +2798,13 @@
         <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F40" t="s">
+        <v>136</v>
+      </c>
+      <c r="G40" t="s">
         <v>137</v>
-      </c>
-      <c r="G40" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2824,18 +2821,18 @@
         <v>80</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F41" t="s">
+        <v>138</v>
+      </c>
+      <c r="G41" t="s">
         <v>139</v>
       </c>
-      <c r="G41" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>141</v>
+      <c r="A42">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2858,7 +2855,7 @@
         <v>80</v>
       </c>
       <c r="G43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2881,7 +2878,7 @@
         <v>80</v>
       </c>
       <c r="G44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2904,7 +2901,7 @@
         <v>80</v>
       </c>
       <c r="G45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2927,7 +2924,7 @@
         <v>80</v>
       </c>
       <c r="G46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2950,7 +2947,7 @@
         <v>80</v>
       </c>
       <c r="G47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2973,7 +2970,7 @@
         <v>80</v>
       </c>
       <c r="G48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2996,7 +2993,7 @@
         <v>80</v>
       </c>
       <c r="G49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3008,15 +3005,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0F6296-D368-4F0B-B654-8C642942CD4C}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
@@ -3028,15 +3025,15 @@
         <v>102</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>143</v>
+      <c r="A2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3044,22 +3041,22 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" t="s">
         <v>145</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>146</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>147</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>148</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>149</v>
-      </c>
-      <c r="G3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3067,22 +3064,22 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" t="s">
         <v>151</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>152</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>153</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>154</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>155</v>
-      </c>
-      <c r="G4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3090,22 +3087,22 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
         <v>157</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>158</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>159</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>160</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>161</v>
-      </c>
-      <c r="G5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3113,22 +3110,22 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
         <v>163</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>164</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>165</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>166</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>167</v>
-      </c>
-      <c r="G6" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3136,22 +3133,22 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" t="s">
         <v>169</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>170</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>171</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>172</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>173</v>
-      </c>
-      <c r="G7" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3159,22 +3156,22 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" t="s">
         <v>175</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>176</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>177</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>178</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>179</v>
-      </c>
-      <c r="G8" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3182,27 +3179,27 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
         <v>181</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>182</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>183</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>184</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>185</v>
       </c>
-      <c r="G9" t="s">
-        <v>186</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>49</v>
+      <c r="A10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -3213,19 +3210,19 @@
         <v>50</v>
       </c>
       <c r="C11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" t="s">
         <v>187</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>188</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>189</v>
       </c>
-      <c r="F11" t="s">
-        <v>190</v>
-      </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -3236,19 +3233,19 @@
         <v>50</v>
       </c>
       <c r="C12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" t="s">
         <v>191</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>192</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>193</v>
       </c>
-      <c r="F12" t="s">
-        <v>194</v>
-      </c>
       <c r="G12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -3259,19 +3256,19 @@
         <v>50</v>
       </c>
       <c r="C13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" t="s">
         <v>195</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>196</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>197</v>
       </c>
-      <c r="F13" t="s">
-        <v>198</v>
-      </c>
       <c r="G13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3282,19 +3279,19 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" t="s">
         <v>199</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>200</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>201</v>
       </c>
-      <c r="F14" t="s">
-        <v>202</v>
-      </c>
       <c r="G14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3305,19 +3302,19 @@
         <v>50</v>
       </c>
       <c r="C15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" t="s">
         <v>203</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>204</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>205</v>
       </c>
-      <c r="F15" t="s">
-        <v>206</v>
-      </c>
       <c r="G15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -3328,19 +3325,19 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16" t="s">
         <v>207</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>208</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>209</v>
       </c>
-      <c r="F16" t="s">
-        <v>210</v>
-      </c>
       <c r="G16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3351,24 +3348,24 @@
         <v>50</v>
       </c>
       <c r="C17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" t="s">
         <v>211</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>212</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>213</v>
       </c>
-      <c r="F17" t="s">
-        <v>214</v>
-      </c>
       <c r="G17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>79</v>
+      <c r="A18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3382,16 +3379,16 @@
         <v>50</v>
       </c>
       <c r="D19" t="s">
+        <v>214</v>
+      </c>
+      <c r="E19" t="s">
         <v>215</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>216</v>
       </c>
-      <c r="F19" t="s">
-        <v>217</v>
-      </c>
       <c r="G19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3405,16 +3402,16 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" t="s">
         <v>218</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>219</v>
       </c>
-      <c r="F20" t="s">
-        <v>220</v>
-      </c>
       <c r="G20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -3428,16 +3425,16 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
+        <v>220</v>
+      </c>
+      <c r="E21" t="s">
         <v>221</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>222</v>
       </c>
-      <c r="F21" t="s">
-        <v>223</v>
-      </c>
       <c r="G21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -3451,16 +3448,16 @@
         <v>50</v>
       </c>
       <c r="D22" t="s">
+        <v>223</v>
+      </c>
+      <c r="E22" t="s">
         <v>224</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>225</v>
       </c>
-      <c r="F22" t="s">
-        <v>226</v>
-      </c>
       <c r="G22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -3474,16 +3471,16 @@
         <v>50</v>
       </c>
       <c r="D23" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" t="s">
         <v>227</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>228</v>
       </c>
-      <c r="F23" t="s">
-        <v>229</v>
-      </c>
       <c r="G23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -3497,16 +3494,16 @@
         <v>50</v>
       </c>
       <c r="D24" t="s">
+        <v>229</v>
+      </c>
+      <c r="E24" t="s">
         <v>230</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>231</v>
       </c>
-      <c r="F24" t="s">
-        <v>232</v>
-      </c>
       <c r="G24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -3520,21 +3517,21 @@
         <v>50</v>
       </c>
       <c r="D25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E25" t="s">
         <v>233</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>234</v>
       </c>
-      <c r="F25" t="s">
-        <v>235</v>
-      </c>
       <c r="G25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>102</v>
+      <c r="A26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -3551,13 +3548,13 @@
         <v>103</v>
       </c>
       <c r="E27" t="s">
+        <v>235</v>
+      </c>
+      <c r="F27" t="s">
         <v>236</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>237</v>
-      </c>
-      <c r="G27" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -3574,13 +3571,13 @@
         <v>103</v>
       </c>
       <c r="E28" t="s">
+        <v>238</v>
+      </c>
+      <c r="F28" t="s">
         <v>239</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>240</v>
-      </c>
-      <c r="G28" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -3597,13 +3594,13 @@
         <v>103</v>
       </c>
       <c r="E29" t="s">
+        <v>241</v>
+      </c>
+      <c r="F29" t="s">
         <v>242</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>243</v>
-      </c>
-      <c r="G29" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -3620,13 +3617,13 @@
         <v>103</v>
       </c>
       <c r="E30" t="s">
+        <v>244</v>
+      </c>
+      <c r="F30" t="s">
         <v>245</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>246</v>
-      </c>
-      <c r="G30" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -3643,13 +3640,13 @@
         <v>103</v>
       </c>
       <c r="E31" t="s">
+        <v>247</v>
+      </c>
+      <c r="F31" t="s">
         <v>248</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>249</v>
-      </c>
-      <c r="G31" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -3666,13 +3663,13 @@
         <v>103</v>
       </c>
       <c r="E32" t="s">
+        <v>250</v>
+      </c>
+      <c r="F32" t="s">
         <v>251</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>252</v>
-      </c>
-      <c r="G32" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -3689,18 +3686,18 @@
         <v>103</v>
       </c>
       <c r="E33" t="s">
+        <v>253</v>
+      </c>
+      <c r="F33" t="s">
         <v>254</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>255</v>
       </c>
-      <c r="G33" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>125</v>
+      <c r="A34">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -3717,13 +3714,13 @@
         <v>80</v>
       </c>
       <c r="E35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F35" t="s">
+        <v>256</v>
+      </c>
+      <c r="G35" t="s">
         <v>257</v>
-      </c>
-      <c r="G35" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -3740,13 +3737,13 @@
         <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F36" t="s">
+        <v>258</v>
+      </c>
+      <c r="G36" t="s">
         <v>259</v>
-      </c>
-      <c r="G36" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -3763,13 +3760,13 @@
         <v>80</v>
       </c>
       <c r="E37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F37" t="s">
+        <v>260</v>
+      </c>
+      <c r="G37" t="s">
         <v>261</v>
-      </c>
-      <c r="G37" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -3786,13 +3783,13 @@
         <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F38" t="s">
+        <v>262</v>
+      </c>
+      <c r="G38" t="s">
         <v>263</v>
-      </c>
-      <c r="G38" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -3809,13 +3806,13 @@
         <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F39" t="s">
+        <v>264</v>
+      </c>
+      <c r="G39" t="s">
         <v>265</v>
-      </c>
-      <c r="G39" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -3832,13 +3829,13 @@
         <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F40" t="s">
+        <v>266</v>
+      </c>
+      <c r="G40" t="s">
         <v>267</v>
-      </c>
-      <c r="G40" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -3855,18 +3852,18 @@
         <v>80</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F41" t="s">
+        <v>268</v>
+      </c>
+      <c r="G41" t="s">
         <v>269</v>
       </c>
-      <c r="G41" t="s">
-        <v>270</v>
-      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>141</v>
+      <c r="A42">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -3889,7 +3886,7 @@
         <v>80</v>
       </c>
       <c r="G43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -3912,7 +3909,7 @@
         <v>80</v>
       </c>
       <c r="G44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -3935,7 +3932,7 @@
         <v>80</v>
       </c>
       <c r="G45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -3958,7 +3955,7 @@
         <v>80</v>
       </c>
       <c r="G46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -3981,7 +3978,7 @@
         <v>80</v>
       </c>
       <c r="G47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4004,7 +4001,7 @@
         <v>80</v>
       </c>
       <c r="G48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -4027,7 +4024,7 @@
         <v>80</v>
       </c>
       <c r="G49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4039,15 +4036,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1605CBBE-8C7A-47C2-83D7-66A660E7ABFF}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
@@ -4059,15 +4056,15 @@
         <v>102</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>143</v>
+      <c r="A2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4075,19 +4072,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" t="s">
         <v>271</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>272</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>273</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>274</v>
-      </c>
-      <c r="G3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -4095,19 +4092,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" t="s">
         <v>276</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>277</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>278</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>279</v>
-      </c>
-      <c r="G4" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -4115,19 +4112,19 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>280</v>
+      </c>
+      <c r="D5" t="s">
         <v>281</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>282</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>283</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>284</v>
-      </c>
-      <c r="G5" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -4135,19 +4132,19 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" t="s">
         <v>286</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>287</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>288</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>289</v>
-      </c>
-      <c r="G6" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -4155,19 +4152,19 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" t="s">
         <v>291</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>292</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>293</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>294</v>
-      </c>
-      <c r="G7" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -4175,19 +4172,19 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D8" t="s">
         <v>296</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>297</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>298</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>299</v>
-      </c>
-      <c r="G8" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -4195,24 +4192,24 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D9" t="s">
         <v>301</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>302</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>303</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>304</v>
       </c>
-      <c r="G9" t="s">
-        <v>305</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>49</v>
+      <c r="A10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -4220,19 +4217,19 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" t="s">
         <v>306</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>307</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>308</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>309</v>
-      </c>
-      <c r="G11" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -4240,19 +4237,19 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D12" t="s">
         <v>311</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>312</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>313</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>314</v>
-      </c>
-      <c r="G12" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -4260,19 +4257,19 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D13" t="s">
         <v>316</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>317</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>318</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>319</v>
-      </c>
-      <c r="G13" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -4280,19 +4277,19 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D14" t="s">
         <v>321</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>322</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>323</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>324</v>
-      </c>
-      <c r="G14" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -4300,19 +4297,19 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
+        <v>325</v>
+      </c>
+      <c r="D15" t="s">
         <v>326</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>327</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>328</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>329</v>
-      </c>
-      <c r="G15" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -4320,19 +4317,19 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
+        <v>330</v>
+      </c>
+      <c r="D16" t="s">
         <v>331</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>332</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>333</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>334</v>
-      </c>
-      <c r="G16" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -4340,24 +4337,24 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
+        <v>335</v>
+      </c>
+      <c r="D17" t="s">
         <v>336</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>337</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>338</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>339</v>
       </c>
-      <c r="G17" t="s">
-        <v>340</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>79</v>
+      <c r="A18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -4368,16 +4365,16 @@
         <v>80</v>
       </c>
       <c r="C19" t="s">
+        <v>340</v>
+      </c>
+      <c r="E19" t="s">
         <v>341</v>
       </c>
-      <c r="E19" t="s">
-        <v>342</v>
-      </c>
       <c r="F19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -4388,16 +4385,16 @@
         <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -4408,16 +4405,16 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -4428,16 +4425,16 @@
         <v>80</v>
       </c>
       <c r="C22" t="s">
+        <v>344</v>
+      </c>
+      <c r="E22" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" t="s">
         <v>345</v>
       </c>
-      <c r="E22" t="s">
-        <v>153</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>346</v>
-      </c>
-      <c r="G22" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -4448,16 +4445,16 @@
         <v>80</v>
       </c>
       <c r="C23" t="s">
+        <v>347</v>
+      </c>
+      <c r="E23" t="s">
         <v>348</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>349</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>350</v>
-      </c>
-      <c r="G23" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -4468,16 +4465,16 @@
         <v>80</v>
       </c>
       <c r="C24" t="s">
+        <v>351</v>
+      </c>
+      <c r="E24" t="s">
         <v>352</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>353</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>354</v>
-      </c>
-      <c r="G24" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4488,21 +4485,21 @@
         <v>80</v>
       </c>
       <c r="C25" t="s">
+        <v>355</v>
+      </c>
+      <c r="E25" t="s">
         <v>356</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>357</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>358</v>
       </c>
-      <c r="G25" t="s">
-        <v>359</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>102</v>
+      <c r="A26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4516,13 +4513,13 @@
         <v>80</v>
       </c>
       <c r="D27" t="s">
+        <v>359</v>
+      </c>
+      <c r="F27" t="s">
+        <v>341</v>
+      </c>
+      <c r="G27" t="s">
         <v>360</v>
-      </c>
-      <c r="F27" t="s">
-        <v>342</v>
-      </c>
-      <c r="G27" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -4536,13 +4533,13 @@
         <v>80</v>
       </c>
       <c r="D28" t="s">
+        <v>361</v>
+      </c>
+      <c r="F28" t="s">
+        <v>341</v>
+      </c>
+      <c r="G28" t="s">
         <v>362</v>
-      </c>
-      <c r="F28" t="s">
-        <v>342</v>
-      </c>
-      <c r="G28" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -4556,13 +4553,13 @@
         <v>80</v>
       </c>
       <c r="D29" t="s">
+        <v>363</v>
+      </c>
+      <c r="F29" t="s">
         <v>364</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>365</v>
-      </c>
-      <c r="G29" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4576,13 +4573,13 @@
         <v>80</v>
       </c>
       <c r="D30" t="s">
+        <v>366</v>
+      </c>
+      <c r="F30" t="s">
         <v>367</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>368</v>
-      </c>
-      <c r="G30" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4596,13 +4593,13 @@
         <v>80</v>
       </c>
       <c r="D31" t="s">
+        <v>369</v>
+      </c>
+      <c r="F31" t="s">
         <v>370</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>371</v>
-      </c>
-      <c r="G31" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4616,13 +4613,13 @@
         <v>80</v>
       </c>
       <c r="D32" t="s">
+        <v>372</v>
+      </c>
+      <c r="F32" t="s">
         <v>373</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>374</v>
-      </c>
-      <c r="G32" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4636,18 +4633,18 @@
         <v>80</v>
       </c>
       <c r="D33" t="s">
+        <v>375</v>
+      </c>
+      <c r="F33" t="s">
         <v>376</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>377</v>
       </c>
-      <c r="G33" t="s">
-        <v>378</v>
-      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>125</v>
+      <c r="A34">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4664,10 +4661,10 @@
         <v>80</v>
       </c>
       <c r="E35" t="s">
+        <v>378</v>
+      </c>
+      <c r="G35" t="s">
         <v>379</v>
-      </c>
-      <c r="G35" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4684,10 +4681,10 @@
         <v>80</v>
       </c>
       <c r="E36" t="s">
+        <v>380</v>
+      </c>
+      <c r="G36" t="s">
         <v>381</v>
-      </c>
-      <c r="G36" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4704,10 +4701,10 @@
         <v>80</v>
       </c>
       <c r="E37" t="s">
+        <v>382</v>
+      </c>
+      <c r="G37" t="s">
         <v>383</v>
-      </c>
-      <c r="G37" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -4724,10 +4721,10 @@
         <v>80</v>
       </c>
       <c r="E38" t="s">
+        <v>384</v>
+      </c>
+      <c r="G38" t="s">
         <v>385</v>
-      </c>
-      <c r="G38" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4744,10 +4741,10 @@
         <v>80</v>
       </c>
       <c r="E39" t="s">
+        <v>386</v>
+      </c>
+      <c r="G39" t="s">
         <v>387</v>
-      </c>
-      <c r="G39" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4764,10 +4761,10 @@
         <v>80</v>
       </c>
       <c r="E40" t="s">
+        <v>388</v>
+      </c>
+      <c r="G40" t="s">
         <v>389</v>
-      </c>
-      <c r="G40" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4784,15 +4781,15 @@
         <v>80</v>
       </c>
       <c r="E41" t="s">
+        <v>390</v>
+      </c>
+      <c r="G41" t="s">
         <v>391</v>
       </c>
-      <c r="G41" t="s">
-        <v>392</v>
-      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>141</v>
+      <c r="A42">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4945,15 +4942,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2746379C-31BF-483F-A87A-C5D7FF3147B4}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
@@ -4965,15 +4962,15 @@
         <v>102</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>143</v>
+      <c r="A2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4981,19 +4978,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>392</v>
+      </c>
+      <c r="D3" t="s">
         <v>393</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>394</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>395</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>396</v>
-      </c>
-      <c r="G3" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -5001,19 +4998,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D4" t="s">
         <v>398</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>399</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>400</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>401</v>
-      </c>
-      <c r="G4" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -5021,19 +5018,19 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D5" t="s">
         <v>403</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>404</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>405</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>406</v>
-      </c>
-      <c r="G5" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -5041,19 +5038,19 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D6" t="s">
         <v>408</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>409</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>410</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>411</v>
-      </c>
-      <c r="G6" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -5061,19 +5058,19 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D7" t="s">
         <v>413</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>414</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>415</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>416</v>
-      </c>
-      <c r="G7" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -5081,19 +5078,19 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" t="s">
         <v>418</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>419</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>420</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>421</v>
-      </c>
-      <c r="G8" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -5101,24 +5098,24 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
+        <v>422</v>
+      </c>
+      <c r="D9" t="s">
         <v>423</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>424</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>425</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>426</v>
       </c>
-      <c r="G9" t="s">
-        <v>427</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>49</v>
+      <c r="A10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -5126,19 +5123,19 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
+        <v>427</v>
+      </c>
+      <c r="D11" t="s">
         <v>428</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>429</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>430</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>431</v>
-      </c>
-      <c r="G11" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -5146,19 +5143,19 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>432</v>
+      </c>
+      <c r="D12" t="s">
         <v>433</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>434</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>435</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>436</v>
-      </c>
-      <c r="G12" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -5166,19 +5163,19 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>437</v>
+      </c>
+      <c r="D13" t="s">
         <v>438</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>439</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>440</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>441</v>
-      </c>
-      <c r="G13" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -5186,19 +5183,19 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
+        <v>442</v>
+      </c>
+      <c r="D14" t="s">
         <v>443</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>444</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>445</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>446</v>
-      </c>
-      <c r="G14" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -5206,19 +5203,19 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
+        <v>447</v>
+      </c>
+      <c r="D15" t="s">
         <v>448</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>449</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>450</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>451</v>
-      </c>
-      <c r="G15" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -5226,19 +5223,19 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
+        <v>452</v>
+      </c>
+      <c r="D16" t="s">
         <v>453</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>454</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>455</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>456</v>
-      </c>
-      <c r="G16" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -5246,24 +5243,24 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
+        <v>457</v>
+      </c>
+      <c r="D17" t="s">
         <v>458</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>459</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>460</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>461</v>
       </c>
-      <c r="G17" t="s">
-        <v>462</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>79</v>
+      <c r="A18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -5274,16 +5271,16 @@
         <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -5294,16 +5291,16 @@
         <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -5314,16 +5311,16 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -5334,16 +5331,16 @@
         <v>80</v>
       </c>
       <c r="C22" t="s">
+        <v>465</v>
+      </c>
+      <c r="E22" t="s">
         <v>466</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>467</v>
       </c>
-      <c r="F22" t="s">
-        <v>468</v>
-      </c>
       <c r="G22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -5354,16 +5351,16 @@
         <v>80</v>
       </c>
       <c r="C23" t="s">
+        <v>468</v>
+      </c>
+      <c r="E23" t="s">
         <v>469</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>470</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>471</v>
-      </c>
-      <c r="G23" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -5374,16 +5371,16 @@
         <v>80</v>
       </c>
       <c r="C24" t="s">
+        <v>472</v>
+      </c>
+      <c r="E24" t="s">
         <v>473</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>474</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>475</v>
-      </c>
-      <c r="G24" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -5394,21 +5391,21 @@
         <v>80</v>
       </c>
       <c r="C25" t="s">
+        <v>476</v>
+      </c>
+      <c r="E25" t="s">
         <v>477</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>478</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>479</v>
       </c>
-      <c r="G25" t="s">
-        <v>480</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>102</v>
+      <c r="A26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -5422,13 +5419,13 @@
         <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -5442,13 +5439,13 @@
         <v>80</v>
       </c>
       <c r="D28" t="s">
+        <v>481</v>
+      </c>
+      <c r="F28" t="s">
         <v>482</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>483</v>
-      </c>
-      <c r="G28" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -5462,13 +5459,13 @@
         <v>80</v>
       </c>
       <c r="D29" t="s">
+        <v>484</v>
+      </c>
+      <c r="F29" t="s">
         <v>485</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>486</v>
-      </c>
-      <c r="G29" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -5482,13 +5479,13 @@
         <v>80</v>
       </c>
       <c r="D30" t="s">
+        <v>487</v>
+      </c>
+      <c r="F30" t="s">
         <v>488</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>489</v>
-      </c>
-      <c r="G30" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -5502,13 +5499,13 @@
         <v>80</v>
       </c>
       <c r="D31" t="s">
+        <v>490</v>
+      </c>
+      <c r="F31" t="s">
         <v>491</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>492</v>
-      </c>
-      <c r="G31" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -5522,13 +5519,13 @@
         <v>80</v>
       </c>
       <c r="D32" t="s">
+        <v>493</v>
+      </c>
+      <c r="F32" t="s">
         <v>494</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>495</v>
-      </c>
-      <c r="G32" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -5542,18 +5539,18 @@
         <v>80</v>
       </c>
       <c r="D33" t="s">
+        <v>496</v>
+      </c>
+      <c r="F33" t="s">
         <v>497</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>498</v>
       </c>
-      <c r="G33" t="s">
-        <v>499</v>
-      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>125</v>
+      <c r="A34">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -5570,10 +5567,10 @@
         <v>80</v>
       </c>
       <c r="E35" t="s">
+        <v>499</v>
+      </c>
+      <c r="G35" t="s">
         <v>500</v>
-      </c>
-      <c r="G35" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -5590,10 +5587,10 @@
         <v>80</v>
       </c>
       <c r="E36" t="s">
+        <v>501</v>
+      </c>
+      <c r="G36" t="s">
         <v>502</v>
-      </c>
-      <c r="G36" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -5610,10 +5607,10 @@
         <v>80</v>
       </c>
       <c r="E37" t="s">
+        <v>503</v>
+      </c>
+      <c r="G37" t="s">
         <v>504</v>
-      </c>
-      <c r="G37" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -5630,10 +5627,10 @@
         <v>80</v>
       </c>
       <c r="E38" t="s">
+        <v>505</v>
+      </c>
+      <c r="G38" t="s">
         <v>506</v>
-      </c>
-      <c r="G38" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -5650,10 +5647,10 @@
         <v>80</v>
       </c>
       <c r="E39" t="s">
+        <v>507</v>
+      </c>
+      <c r="G39" t="s">
         <v>508</v>
-      </c>
-      <c r="G39" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -5670,10 +5667,10 @@
         <v>80</v>
       </c>
       <c r="E40" t="s">
+        <v>509</v>
+      </c>
+      <c r="G40" t="s">
         <v>510</v>
-      </c>
-      <c r="G40" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -5690,15 +5687,15 @@
         <v>80</v>
       </c>
       <c r="E41" t="s">
+        <v>511</v>
+      </c>
+      <c r="G41" t="s">
         <v>512</v>
       </c>
-      <c r="G41" t="s">
-        <v>513</v>
-      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>141</v>
+      <c r="A42">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>